<commit_message>
excel tests_urls_tips_final with status automation
</commit_message>
<xml_diff>
--- a/manual/tests_urls_tips_final.xlsx
+++ b/manual/tests_urls_tips_final.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imane\Documents\DataAut\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE766371-C05A-42E8-8702-D9F6D9E8AA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-7455" yWindow="-75" windowWidth="25650" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$180</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$182</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="506">
   <si>
     <t>country</t>
   </si>
@@ -1541,15 +1535,51 @@
   <si>
     <t>https://data.gov.hk/en-data/dataset/hk-dh-chpsebcddr-novel-infectious-agent</t>
   </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>automated</t>
+  </si>
+  <si>
+    <t>facebook information</t>
+  </si>
+  <si>
+    <t>twitter information</t>
+  </si>
+  <si>
+    <t>to be implemented</t>
+  </si>
+  <si>
+    <t>not yet implemented</t>
+  </si>
+  <si>
+    <t>telegram page</t>
+  </si>
+  <si>
+    <t>stauts_with_automatization</t>
+  </si>
+  <si>
+    <t>We're fixing errors in python</t>
+  </si>
+  <si>
+    <t>We need to review the new link</t>
+  </si>
+  <si>
+    <t>withuot info, We need to check with new links</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$]dddd\,\ mmmm\ d\,\ yyyy;@" x16r2:formatCode16="[$-en-CH,1]dddd\,\ mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$]dddd\,\ mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1721,6 +1751,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1767,7 +1806,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1819,11 +1858,12 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1883,7 +1923,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1918,7 +1958,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2095,24 +2135,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K182"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -2126,7 +2166,7 @@
     <col min="11" max="11" width="80.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2160,8 +2200,11 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="41" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
@@ -2187,8 +2230,11 @@
       <c r="K2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="19" t="s">
         <v>259</v>
       </c>
@@ -2211,8 +2257,11 @@
       <c r="H3" s="29" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="26" t="s">
         <v>15</v>
       </c>
@@ -2228,8 +2277,11 @@
       <c r="H4" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="26" t="s">
         <v>18</v>
       </c>
@@ -2245,8 +2297,11 @@
       <c r="H5" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="37" t="s">
         <v>260</v>
       </c>
@@ -2264,8 +2319,11 @@
         <v>473</v>
       </c>
       <c r="I6" s="36"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="26" t="s">
         <v>19</v>
       </c>
@@ -2297,8 +2355,11 @@
       <c r="K7" s="3" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="26" t="s">
         <v>20</v>
       </c>
@@ -2319,8 +2380,11 @@
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="26" t="s">
         <v>25</v>
       </c>
@@ -2339,8 +2403,11 @@
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="26" t="s">
         <v>27</v>
       </c>
@@ -2360,8 +2427,11 @@
         <v>31</v>
       </c>
       <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="26" t="s">
         <v>32</v>
       </c>
@@ -2378,8 +2448,11 @@
         <v>35</v>
       </c>
       <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="26" t="s">
         <v>36</v>
       </c>
@@ -2399,8 +2472,11 @@
         <v>427</v>
       </c>
       <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="40" t="s">
         <v>38</v>
       </c>
@@ -2417,8 +2493,11 @@
       <c r="K13" s="8" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>326</v>
       </c>
@@ -2434,8 +2513,11 @@
       <c r="K14" s="8" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="20" t="s">
         <v>39</v>
       </c>
@@ -2459,8 +2541,11 @@
       <c r="K15" s="8" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="23" t="s">
         <v>42</v>
       </c>
@@ -2479,8 +2564,11 @@
       <c r="K16" s="8" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="16" t="s">
         <v>261</v>
       </c>
@@ -2498,8 +2586,11 @@
       <c r="K17" s="8" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="26" t="s">
         <v>44</v>
       </c>
@@ -2515,8 +2606,11 @@
       <c r="H18" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="26" t="s">
         <v>45</v>
       </c>
@@ -2536,8 +2630,11 @@
       <c r="H19" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="16" t="s">
         <v>262</v>
       </c>
@@ -2553,8 +2650,11 @@
       <c r="K20" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="16" t="s">
         <v>263</v>
       </c>
@@ -2573,8 +2673,11 @@
       <c r="K21" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="26" t="s">
         <v>47</v>
       </c>
@@ -2591,8 +2694,11 @@
         <v>14</v>
       </c>
       <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="26" t="s">
         <v>50</v>
       </c>
@@ -2608,8 +2714,11 @@
       <c r="H23" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="39" t="s">
         <v>51</v>
       </c>
@@ -2625,8 +2734,11 @@
       </c>
       <c r="H24" s="4"/>
       <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="26" t="s">
         <v>264</v>
       </c>
@@ -2643,8 +2755,11 @@
         <v>17</v>
       </c>
       <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="26" t="s">
         <v>52</v>
       </c>
@@ -2661,8 +2776,11 @@
         <v>255</v>
       </c>
       <c r="I26"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="26" t="s">
         <v>54</v>
       </c>
@@ -2678,8 +2796,11 @@
       <c r="H27" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="26" t="s">
         <v>56</v>
       </c>
@@ -2695,8 +2816,11 @@
       <c r="H28" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="16" t="s">
         <v>266</v>
       </c>
@@ -2710,8 +2834,11 @@
         <v>388</v>
       </c>
       <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="26" t="s">
         <v>57</v>
       </c>
@@ -2727,8 +2854,11 @@
       <c r="H30" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="26" t="s">
         <v>58</v>
       </c>
@@ -2745,8 +2875,11 @@
         <v>17</v>
       </c>
       <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="26" t="s">
         <v>59</v>
       </c>
@@ -2762,8 +2895,11 @@
       <c r="H32" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="26" t="s">
         <v>61</v>
       </c>
@@ -2779,8 +2915,11 @@
       <c r="H33" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="26" t="s">
         <v>63</v>
       </c>
@@ -2796,8 +2935,11 @@
       <c r="H34" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="26" t="s">
         <v>64</v>
       </c>
@@ -2821,8 +2963,11 @@
         <v>60556</v>
       </c>
       <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="26" t="s">
         <v>68</v>
       </c>
@@ -2842,8 +2987,11 @@
         <v>71</v>
       </c>
       <c r="K36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="26" t="s">
         <v>72</v>
       </c>
@@ -2859,8 +3007,11 @@
       <c r="H37" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="19" t="s">
         <v>73</v>
       </c>
@@ -2881,8 +3032,11 @@
       <c r="K38" s="8" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="26" t="s">
         <v>75</v>
       </c>
@@ -2898,8 +3052,11 @@
       <c r="H39" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="26" t="s">
         <v>77</v>
       </c>
@@ -2919,8 +3076,11 @@
         <v>394</v>
       </c>
       <c r="K40" s="8"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="19" t="s">
         <v>268</v>
       </c>
@@ -2942,8 +3102,11 @@
       <c r="K41" s="8" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="19" t="s">
         <v>79</v>
       </c>
@@ -2963,8 +3126,11 @@
       <c r="K42" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="26" t="s">
         <v>82</v>
       </c>
@@ -2981,8 +3147,11 @@
         <v>85</v>
       </c>
       <c r="K43" s="7"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="26" t="s">
         <v>86</v>
       </c>
@@ -2998,8 +3167,11 @@
       <c r="H44" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="23" t="s">
         <v>88</v>
       </c>
@@ -3021,8 +3193,11 @@
       <c r="K45" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="26" t="s">
         <v>89</v>
       </c>
@@ -3038,8 +3213,11 @@
       <c r="H46" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="16" t="s">
         <v>270</v>
       </c>
@@ -3053,8 +3231,11 @@
         <v>384</v>
       </c>
       <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="19" t="s">
         <v>271</v>
       </c>
@@ -3071,8 +3252,11 @@
       <c r="K48" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="26" t="s">
         <v>90</v>
       </c>
@@ -3089,8 +3273,11 @@
         <v>429</v>
       </c>
       <c r="I49"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="26" t="s">
         <v>92</v>
       </c>
@@ -3106,8 +3293,11 @@
       <c r="H50" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="35" t="s">
         <v>93</v>
       </c>
@@ -3126,8 +3316,11 @@
       <c r="K51" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L51" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="10" customFormat="1">
       <c r="A52" s="26" t="s">
         <v>98</v>
       </c>
@@ -3149,8 +3342,11 @@
       <c r="I52" s="1"/>
       <c r="J52" s="2"/>
       <c r="K52"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="26" t="s">
         <v>100</v>
       </c>
@@ -3166,8 +3362,11 @@
       <c r="H53" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="26" t="s">
         <v>101</v>
       </c>
@@ -3187,8 +3386,11 @@
         <v>14</v>
       </c>
       <c r="I54" s="36"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="26" t="s">
         <v>104</v>
       </c>
@@ -3204,8 +3406,11 @@
       <c r="H55" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="26" t="s">
         <v>105</v>
       </c>
@@ -3221,8 +3426,11 @@
       <c r="H56" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="26" t="s">
         <v>106</v>
       </c>
@@ -3239,8 +3447,11 @@
       <c r="H57" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="16" t="s">
         <v>272</v>
       </c>
@@ -3256,8 +3467,11 @@
       <c r="K58" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="23" t="s">
         <v>108</v>
       </c>
@@ -3280,8 +3494,11 @@
         <v>406</v>
       </c>
       <c r="I59" s="30"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="26" t="s">
         <v>110</v>
       </c>
@@ -3299,8 +3516,11 @@
         <v>121</v>
       </c>
       <c r="K60" s="7"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>273</v>
       </c>
@@ -3315,8 +3535,11 @@
         <v>388</v>
       </c>
       <c r="K61" s="7"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="26" t="s">
         <v>111</v>
       </c>
@@ -3332,8 +3555,11 @@
       <c r="H62" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>274</v>
       </c>
@@ -3347,8 +3573,11 @@
         <v>388</v>
       </c>
       <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>275</v>
       </c>
@@ -3365,8 +3594,11 @@
       <c r="K64" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="26" t="s">
         <v>112</v>
       </c>
@@ -3382,8 +3614,11 @@
       <c r="H65" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="23" t="s">
         <v>113</v>
       </c>
@@ -3400,8 +3635,11 @@
       <c r="K66" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" s="26" t="s">
         <v>115</v>
       </c>
@@ -3418,8 +3656,11 @@
       <c r="H67" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>276</v>
       </c>
@@ -3432,8 +3673,11 @@
       <c r="E68" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" s="10" t="s">
         <v>277</v>
       </c>
@@ -3452,8 +3696,11 @@
       <c r="K69" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" s="26" t="s">
         <v>116</v>
       </c>
@@ -3469,8 +3716,11 @@
       <c r="H70" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" s="26" t="s">
         <v>117</v>
       </c>
@@ -3486,8 +3736,11 @@
       <c r="H71" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>278</v>
       </c>
@@ -3501,8 +3754,11 @@
         <v>388</v>
       </c>
       <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" s="10" t="s">
         <v>279</v>
       </c>
@@ -3516,8 +3772,11 @@
         <v>465</v>
       </c>
       <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="10" t="s">
         <v>330</v>
       </c>
@@ -3537,8 +3796,11 @@
       <c r="K74" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" s="26" t="s">
         <v>119</v>
       </c>
@@ -3555,8 +3817,11 @@
         <v>121</v>
       </c>
       <c r="K75" s="7"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="17" t="s">
         <v>122</v>
       </c>
@@ -3574,8 +3839,11 @@
       <c r="K76" s="8" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" s="26" t="s">
         <v>123</v>
       </c>
@@ -3598,8 +3866,11 @@
       <c r="H77" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="26" t="s">
         <v>127</v>
       </c>
@@ -3617,8 +3888,11 @@
         <v>129</v>
       </c>
       <c r="K78" s="7"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" s="16" t="s">
         <v>282</v>
       </c>
@@ -3635,8 +3909,11 @@
       <c r="K79" s="8" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" s="16" t="s">
         <v>335</v>
       </c>
@@ -3653,8 +3930,11 @@
       <c r="K80" s="8" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="26" t="s">
         <v>283</v>
       </c>
@@ -3672,8 +3952,11 @@
         <v>17</v>
       </c>
       <c r="K81" s="7"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="16" t="s">
         <v>284</v>
       </c>
@@ -3689,8 +3972,11 @@
       <c r="K82" s="8" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="26" t="s">
         <v>130</v>
       </c>
@@ -3711,8 +3997,11 @@
         <v>254</v>
       </c>
       <c r="K83" s="7"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="19" t="s">
         <v>285</v>
       </c>
@@ -3737,8 +4026,11 @@
       <c r="K84" s="8" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" s="16" t="s">
         <v>286</v>
       </c>
@@ -3755,8 +4047,11 @@
       <c r="K85" s="8" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" s="26" t="s">
         <v>133</v>
       </c>
@@ -3774,8 +4069,11 @@
         <v>135</v>
       </c>
       <c r="K86" s="7"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="35" t="s">
         <v>136</v>
       </c>
@@ -3791,8 +4089,11 @@
       <c r="K87" s="8" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="26" t="s">
         <v>138</v>
       </c>
@@ -3808,8 +4109,11 @@
       <c r="H88" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="16" t="s">
         <v>287</v>
       </c>
@@ -3826,8 +4130,11 @@
       <c r="K89" s="8" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="22" t="s">
         <v>139</v>
       </c>
@@ -3844,8 +4151,11 @@
       <c r="H90"/>
       <c r="I90"/>
       <c r="K90" s="7"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" s="27" t="s">
         <v>289</v>
       </c>
@@ -3863,8 +4173,11 @@
       </c>
       <c r="I91"/>
       <c r="K91" s="7"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="26" t="s">
         <v>141</v>
       </c>
@@ -3882,8 +4195,11 @@
         <v>121</v>
       </c>
       <c r="K92" s="7"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="26" t="s">
         <v>143</v>
       </c>
@@ -3905,8 +4221,11 @@
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="26" t="s">
         <v>146</v>
       </c>
@@ -3922,8 +4241,11 @@
       <c r="H94" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="26" t="s">
         <v>147</v>
       </c>
@@ -3939,8 +4261,11 @@
       <c r="H95" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="26" t="s">
         <v>148</v>
       </c>
@@ -3956,8 +4281,11 @@
       <c r="H96" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" s="38" t="s">
         <v>149</v>
       </c>
@@ -3975,8 +4303,11 @@
       </c>
       <c r="I97" s="36"/>
       <c r="K97" s="8"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="23" t="s">
         <v>150</v>
       </c>
@@ -3996,8 +4327,11 @@
       <c r="K98" s="32" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" s="26" t="s">
         <v>152</v>
       </c>
@@ -4013,8 +4347,11 @@
       <c r="H99" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" s="16" t="s">
         <v>290</v>
       </c>
@@ -4025,8 +4362,11 @@
         <v>388</v>
       </c>
       <c r="H100" s="4"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L100" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" s="26" t="s">
         <v>153</v>
       </c>
@@ -4042,8 +4382,11 @@
       <c r="H101" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L101" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" s="14" t="s">
         <v>291</v>
       </c>
@@ -4060,8 +4403,11 @@
       <c r="K102" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L102" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" s="26" t="s">
         <v>154</v>
       </c>
@@ -4077,8 +4423,11 @@
       <c r="H103" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L103" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="35" t="s">
         <v>155</v>
       </c>
@@ -4097,8 +4446,11 @@
       <c r="K104" s="8" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="26" t="s">
         <v>157</v>
       </c>
@@ -4114,8 +4466,11 @@
       <c r="H105" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L105" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" s="26" t="s">
         <v>158</v>
       </c>
@@ -4131,8 +4486,11 @@
       <c r="H106" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L106" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" s="23" t="s">
         <v>159</v>
       </c>
@@ -4150,8 +4508,11 @@
       <c r="K107" s="8" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L107" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" s="23" t="s">
         <v>476</v>
       </c>
@@ -4168,8 +4529,11 @@
       <c r="H108"/>
       <c r="I108"/>
       <c r="K108" s="8"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L108" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" s="19" t="s">
         <v>337</v>
       </c>
@@ -4186,8 +4550,11 @@
       <c r="H109"/>
       <c r="I109"/>
       <c r="K109" s="7"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L109" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" s="26" t="s">
         <v>161</v>
       </c>
@@ -4203,8 +4570,11 @@
       <c r="H110" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L110" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" s="26" t="s">
         <v>162</v>
       </c>
@@ -4220,8 +4590,11 @@
       <c r="H111" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L111" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" s="35" t="s">
         <v>163</v>
       </c>
@@ -4237,8 +4610,11 @@
       <c r="K112" s="8" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L112" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" s="26" t="s">
         <v>165</v>
       </c>
@@ -4254,8 +4630,11 @@
       <c r="H113" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L113" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" s="26" t="s">
         <v>166</v>
       </c>
@@ -4273,8 +4652,11 @@
       </c>
       <c r="I114" s="5"/>
       <c r="J114" s="6"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L114" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" s="14" t="s">
         <v>292</v>
       </c>
@@ -4293,8 +4675,11 @@
       <c r="K115" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L115" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" s="26" t="s">
         <v>168</v>
       </c>
@@ -4312,8 +4697,11 @@
       <c r="H116" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L116" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" s="26" t="s">
         <v>171</v>
       </c>
@@ -4331,8 +4719,11 @@
         <v>17</v>
       </c>
       <c r="K117" s="7"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L117" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" s="26" t="s">
         <v>173</v>
       </c>
@@ -4348,8 +4739,11 @@
       <c r="H118" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L118" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" s="26" t="s">
         <v>174</v>
       </c>
@@ -4365,8 +4759,11 @@
       <c r="H119" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L119" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" s="23" t="s">
         <v>294</v>
       </c>
@@ -4384,8 +4781,11 @@
         <v>121</v>
       </c>
       <c r="I120" s="36"/>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L120" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" s="26" t="s">
         <v>175</v>
       </c>
@@ -4403,8 +4803,11 @@
       <c r="H121" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L121" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="26" t="s">
         <v>176</v>
       </c>
@@ -4421,8 +4824,11 @@
         <v>17</v>
       </c>
       <c r="K122" s="7"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L122" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" s="16" t="s">
         <v>295</v>
       </c>
@@ -4436,8 +4842,11 @@
         <v>388</v>
       </c>
       <c r="K123" s="7"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L123" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" s="26" t="s">
         <v>179</v>
       </c>
@@ -4455,8 +4864,11 @@
         <v>17</v>
       </c>
       <c r="I124" s="36"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L124" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" s="22" t="s">
         <v>181</v>
       </c>
@@ -4472,8 +4884,11 @@
       <c r="K125" s="8" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L125" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" s="33" t="s">
         <v>296</v>
       </c>
@@ -4492,8 +4907,11 @@
       </c>
       <c r="I126" s="36"/>
       <c r="K126" s="7"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L126" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" s="10" t="s">
         <v>298</v>
       </c>
@@ -4507,8 +4925,11 @@
         <v>385</v>
       </c>
       <c r="K127" s="7"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L127" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" s="26" t="s">
         <v>182</v>
       </c>
@@ -4532,8 +4953,11 @@
         <v>187</v>
       </c>
       <c r="I128" s="4"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L128" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" s="23" t="s">
         <v>188</v>
       </c>
@@ -4549,8 +4973,11 @@
       </c>
       <c r="F129" s="3"/>
       <c r="I129" s="4"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L129" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" s="35" t="s">
         <v>190</v>
       </c>
@@ -4569,8 +4996,11 @@
       <c r="K130" s="8" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L130" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" s="26" t="s">
         <v>192</v>
       </c>
@@ -4587,8 +5017,11 @@
       <c r="H131" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L131" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" s="26" t="s">
         <v>194</v>
       </c>
@@ -4606,8 +5039,11 @@
         <v>17</v>
       </c>
       <c r="I132" s="36"/>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L132" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" s="26" t="s">
         <v>197</v>
       </c>
@@ -4623,8 +5059,11 @@
       <c r="H133" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L133" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="A134" s="23" t="s">
         <v>199</v>
       </c>
@@ -4647,8 +5086,11 @@
       <c r="K134" s="8" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L134" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" s="24" t="s">
         <v>299</v>
       </c>
@@ -4669,8 +5111,11 @@
       <c r="K135" s="8" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L135" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" s="26" t="s">
         <v>203</v>
       </c>
@@ -4686,8 +5131,11 @@
       <c r="H136" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L136" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="A137" t="s">
         <v>301</v>
       </c>
@@ -4702,8 +5150,11 @@
         <v>388</v>
       </c>
       <c r="H137" s="4"/>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L137" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" s="26" t="s">
         <v>257</v>
       </c>
@@ -4721,8 +5172,11 @@
         <v>17</v>
       </c>
       <c r="I138" s="36"/>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L138" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
       <c r="A139" t="s">
         <v>302</v>
       </c>
@@ -4739,8 +5193,11 @@
       <c r="K139" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L139" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
       <c r="A140" t="s">
         <v>304</v>
       </c>
@@ -4757,8 +5214,11 @@
       <c r="K140" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L140" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
       <c r="A141" s="26" t="s">
         <v>204</v>
       </c>
@@ -4774,8 +5234,11 @@
       <c r="H141" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L141" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" s="35" t="s">
         <v>206</v>
       </c>
@@ -4791,8 +5254,11 @@
       <c r="K142" s="8" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L142" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
       <c r="A143" s="23" t="s">
         <v>207</v>
       </c>
@@ -4809,8 +5275,11 @@
       <c r="H143" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L143" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144" s="26" t="s">
         <v>208</v>
       </c>
@@ -4826,8 +5295,11 @@
       <c r="H144" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L144" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
       <c r="A145" s="26" t="s">
         <v>209</v>
       </c>
@@ -4844,8 +5316,11 @@
       <c r="H145" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L145" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" s="26" t="s">
         <v>212</v>
       </c>
@@ -4861,8 +5336,11 @@
       <c r="H146" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L146" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
       <c r="A147" s="26" t="s">
         <v>213</v>
       </c>
@@ -4878,8 +5356,11 @@
       <c r="H147" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L147" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" s="26" t="s">
         <v>215</v>
       </c>
@@ -4897,8 +5378,11 @@
         <v>17</v>
       </c>
       <c r="K148" s="7"/>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L148" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
       <c r="A149" s="26" t="s">
         <v>217</v>
       </c>
@@ -4916,8 +5400,11 @@
         <v>121</v>
       </c>
       <c r="K149" s="7"/>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L149" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
       <c r="A150" s="26" t="s">
         <v>219</v>
       </c>
@@ -4934,8 +5421,11 @@
         <v>433</v>
       </c>
       <c r="K150" s="7"/>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L150" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
       <c r="A151" s="26" t="s">
         <v>220</v>
       </c>
@@ -4951,8 +5441,11 @@
       <c r="H151" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L151" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
       <c r="A152" s="26" t="s">
         <v>306</v>
       </c>
@@ -4969,8 +5462,11 @@
       <c r="H152" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L152" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
       <c r="A153" s="26" t="s">
         <v>221</v>
       </c>
@@ -4986,8 +5482,11 @@
       <c r="H153" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L153" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
       <c r="A154" s="16" t="s">
         <v>309</v>
       </c>
@@ -5004,8 +5503,11 @@
       <c r="K154" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L154" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
       <c r="A155" s="27" t="s">
         <v>310</v>
       </c>
@@ -5021,8 +5523,11 @@
       <c r="H155" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L155" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
       <c r="A156" s="26" t="s">
         <v>222</v>
       </c>
@@ -5038,8 +5543,11 @@
       <c r="H156" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L156" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
       <c r="A157" s="16" t="s">
         <v>312</v>
       </c>
@@ -5056,8 +5564,11 @@
       <c r="K157" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L157" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
       <c r="A158" s="26" t="s">
         <v>223</v>
       </c>
@@ -5077,8 +5588,11 @@
       </c>
       <c r="I158" s="36"/>
       <c r="K158" s="7"/>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L158" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
       <c r="A159" s="35" t="s">
         <v>224</v>
       </c>
@@ -5098,8 +5612,11 @@
       <c r="I159" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L159" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
       <c r="A160" s="17" t="s">
         <v>313</v>
       </c>
@@ -5112,8 +5629,11 @@
       <c r="E160" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L160" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
       <c r="A161" s="26" t="s">
         <v>228</v>
       </c>
@@ -5130,8 +5650,11 @@
         <v>230</v>
       </c>
       <c r="K161" s="7"/>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L161" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>315</v>
       </c>
@@ -5145,8 +5668,11 @@
         <v>384</v>
       </c>
       <c r="K162" s="7"/>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L162" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
       <c r="A163" s="26" t="s">
         <v>231</v>
       </c>
@@ -5162,8 +5688,11 @@
       <c r="H163" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L163" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12">
       <c r="A164" s="26" t="s">
         <v>233</v>
       </c>
@@ -5179,8 +5708,11 @@
       <c r="H164" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L164" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12">
       <c r="A165" s="10" t="s">
         <v>318</v>
       </c>
@@ -5194,8 +5726,11 @@
         <v>380</v>
       </c>
       <c r="H165" s="4"/>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L165" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12">
       <c r="A166" s="26" t="s">
         <v>234</v>
       </c>
@@ -5211,8 +5746,11 @@
       <c r="H166" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L166" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12">
       <c r="A167" s="26" t="s">
         <v>235</v>
       </c>
@@ -5229,8 +5767,11 @@
         <v>363</v>
       </c>
       <c r="K167" s="7"/>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L167" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
       <c r="A168" s="26" t="s">
         <v>237</v>
       </c>
@@ -5246,8 +5787,11 @@
       <c r="H168" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L168" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
       <c r="A169" s="26" t="s">
         <v>238</v>
       </c>
@@ -5265,8 +5809,11 @@
         <v>17</v>
       </c>
       <c r="I169" s="36"/>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L169" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
       <c r="A170" s="26" t="s">
         <v>240</v>
       </c>
@@ -5282,8 +5829,11 @@
       <c r="H170" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L170" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
       <c r="A171" s="33" t="s">
         <v>319</v>
       </c>
@@ -5299,8 +5849,11 @@
       <c r="H171" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L171" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
       <c r="A172" s="26" t="s">
         <v>242</v>
       </c>
@@ -5316,8 +5869,11 @@
       <c r="H172" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L172" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
       <c r="A173" s="23" t="s">
         <v>244</v>
       </c>
@@ -5342,8 +5898,11 @@
       <c r="K173" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L173" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
       <c r="A174" s="26" t="s">
         <v>246</v>
       </c>
@@ -5362,8 +5921,11 @@
       <c r="H174" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L174" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
       <c r="A175" t="s">
         <v>321</v>
       </c>
@@ -5376,8 +5938,11 @@
       <c r="E175" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L175" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
       <c r="A176" t="s">
         <v>324</v>
       </c>
@@ -5390,8 +5955,11 @@
       <c r="E176" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L176" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
       <c r="A177" t="s">
         <v>325</v>
       </c>
@@ -5407,8 +5975,11 @@
       <c r="K177" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L177" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
       <c r="A178" s="26" t="s">
         <v>357</v>
       </c>
@@ -5424,8 +5995,11 @@
       <c r="H178" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L178" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
       <c r="A179" s="26" t="s">
         <v>252</v>
       </c>
@@ -5441,8 +6015,11 @@
       <c r="H179" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L179" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12">
       <c r="A180" s="26" t="s">
         <v>253</v>
       </c>
@@ -5458,49 +6035,52 @@
       <c r="H180" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L180" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
       <c r="H181" s="4"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12">
       <c r="H182" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K180" xr:uid="{4C40DBC0-690F-4D78-B3A1-0E4146828A8F}"/>
+  <autoFilter ref="A1:L182"/>
   <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1" xr:uid="{0118D932-9AD8-4554-AE1F-C83EE2EAC33A}"/>
-    <hyperlink ref="F35" r:id="rId2" xr:uid="{836EEE4A-B363-4967-9045-CF7082EE9BEC}"/>
-    <hyperlink ref="C57" r:id="rId3" xr:uid="{88895BF1-FC1C-4868-9448-9B65CB7829B6}"/>
-    <hyperlink ref="C67" r:id="rId4" xr:uid="{29CF171A-54A2-496F-91B3-BD2A2F665785}"/>
-    <hyperlink ref="C77" r:id="rId5" xr:uid="{8A70436A-132C-4ED4-AB39-E93EEE6D84D3}"/>
-    <hyperlink ref="F77" r:id="rId6" xr:uid="{70FDC53C-DAAC-4DE0-B08E-D2A2CC771405}"/>
-    <hyperlink ref="C81" r:id="rId7" xr:uid="{FACC6A3D-D41A-4EFE-A2CC-0E06E5E8C301}"/>
-    <hyperlink ref="F83" r:id="rId8" xr:uid="{C200101E-F6B8-4F3C-8195-BF8B11BB991A}"/>
-    <hyperlink ref="C128" r:id="rId9" xr:uid="{31A5B51B-DB3A-41AF-A103-3FBB5D01653E}"/>
-    <hyperlink ref="F128" r:id="rId10" xr:uid="{4CB7F428-2056-446B-B0CE-9E58C51B6761}"/>
-    <hyperlink ref="C131" r:id="rId11" xr:uid="{097CF2DF-83FE-44C0-9AF5-0DC754174E12}"/>
-    <hyperlink ref="C145" r:id="rId12" xr:uid="{D093B157-0BE3-443A-91C1-4846D4553C51}"/>
-    <hyperlink ref="C149" r:id="rId13" xr:uid="{F0B61437-B8AD-432D-9E10-237C9726106F}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{96EA50E3-B114-4411-A590-E0CDCCCD3DF0}"/>
-    <hyperlink ref="C24" r:id="rId15" xr:uid="{AE93467C-D373-4E3A-B8CA-D7D2B796927D}"/>
-    <hyperlink ref="C42" r:id="rId16" xr:uid="{56BDF0AB-1125-407A-B774-9CE2AA145662}"/>
-    <hyperlink ref="C61" r:id="rId17" xr:uid="{40CE8585-ABDA-4AE8-A131-5B2B11C82420}"/>
-    <hyperlink ref="C76" r:id="rId18" xr:uid="{B76AFDAC-232E-44F0-9DBE-F36C7214731C}"/>
-    <hyperlink ref="C79" r:id="rId19" xr:uid="{C27E6A35-F9F5-4EB2-88C9-374088C4D387}"/>
-    <hyperlink ref="C90" r:id="rId20" xr:uid="{25A01D12-8936-4EED-ABBC-42B2A4DE84C7}"/>
-    <hyperlink ref="C104" r:id="rId21" xr:uid="{5B530FD3-57D2-4A2D-AD11-8AEE642D59D8}"/>
-    <hyperlink ref="C130" r:id="rId22" xr:uid="{70901922-36A3-45BA-8B10-238F0FD22F94}"/>
-    <hyperlink ref="C129" r:id="rId23" xr:uid="{207047A4-D146-4C92-B816-D563D3BFC01E}"/>
-    <hyperlink ref="C135" r:id="rId24" display="https://www.rospotrebnadzor.ru/search/index.php?tags=&amp;q=%C8%ED%F4%EE%F0%EC%E0%F6%E8%EE%ED%ED%FB%E9+%E1%FE%EB%EB%E5%F2%E5%ED%FC+%EE+%F1%E8%F2%F3%E0%F6%E8%E8+%E8+%EF%F0%E8%ED%E8%EC%E0%E5%EC%FB%F5+%EC%E5%F0%E0%F5+%EF%EE+%ED%E5%E4%EE%EF%F3%F9%E5%ED%E8%FE+%F0%E0%F1%EF%F0%EE%F1%F2%F0%E0%ED%E5%ED%E8%FF+%E7%E0%E1%EE%EB%E5%E2%E0%ED%E8%E9%2C+%E2%FB%E7%E2%E0%ED%ED%FB%F5+%ED%EE%E2%FB%EC+%EA%EE%F0%EE%ED%E0%E2%E8%F0%F3%F1%EE%EC&amp;where=&amp;how=d&amp;from=&amp;to=" xr:uid="{E26D6354-180F-4F00-BD42-13B0CFDBF19A}"/>
-    <hyperlink ref="C134" r:id="rId25" xr:uid="{9F22A71E-0370-446C-B98C-6BB1D19EE35B}"/>
-    <hyperlink ref="C159" r:id="rId26" xr:uid="{BA8DB0DA-0D8A-45EA-89FD-4A0C15B115CB}"/>
-    <hyperlink ref="F173" r:id="rId27" display="https://www.gub.uy/sistema-nacional-emergencias/comunicacion/comunicados/informe-situacion-sobre-coronavirus-covid-19-uruguay-DATE" xr:uid="{3BC7BC8F-BD43-4B9F-8C4C-4E0B11188BA4}"/>
-    <hyperlink ref="C7:K7" r:id="rId28" display="https://www.argentina.gob.ar/coronavirus/informes-diarios/reportes/diciembre2020" xr:uid="{7E5A1A65-8860-4281-B5FC-9A987A840440}"/>
-    <hyperlink ref="C2" r:id="rId29" location="/" display="http://covid.moph-dw.org/ - /" xr:uid="{1FDD1263-C9CC-4266-8257-DEB07627BB37}"/>
-    <hyperlink ref="C107" r:id="rId30" xr:uid="{52AB7E88-15B4-46E3-A274-F4E647E854E0}"/>
-    <hyperlink ref="C124" r:id="rId31" xr:uid="{5B5C6512-3445-4A16-B5B8-06BB467FE458}"/>
-    <hyperlink ref="C126" r:id="rId32" xr:uid="{46A63B76-7A05-4871-B89F-A799D255C8A2}"/>
-    <hyperlink ref="C138" r:id="rId33" xr:uid="{0DD9AC4C-E2CF-4AA8-BFE8-8EF3F7C00A24}"/>
+    <hyperlink ref="C35" r:id="rId1"/>
+    <hyperlink ref="F35" r:id="rId2"/>
+    <hyperlink ref="C57" r:id="rId3"/>
+    <hyperlink ref="C67" r:id="rId4"/>
+    <hyperlink ref="C77" r:id="rId5"/>
+    <hyperlink ref="F77" r:id="rId6"/>
+    <hyperlink ref="C81" r:id="rId7"/>
+    <hyperlink ref="F83" r:id="rId8"/>
+    <hyperlink ref="C128" r:id="rId9"/>
+    <hyperlink ref="F128" r:id="rId10"/>
+    <hyperlink ref="C131" r:id="rId11"/>
+    <hyperlink ref="C145" r:id="rId12"/>
+    <hyperlink ref="C149" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId14"/>
+    <hyperlink ref="C24" r:id="rId15"/>
+    <hyperlink ref="C42" r:id="rId16"/>
+    <hyperlink ref="C61" r:id="rId17"/>
+    <hyperlink ref="C76" r:id="rId18"/>
+    <hyperlink ref="C79" r:id="rId19"/>
+    <hyperlink ref="C90" r:id="rId20"/>
+    <hyperlink ref="C104" r:id="rId21"/>
+    <hyperlink ref="C130" r:id="rId22"/>
+    <hyperlink ref="C129" r:id="rId23"/>
+    <hyperlink ref="C135" r:id="rId24" display="https://www.rospotrebnadzor.ru/search/index.php?tags=&amp;q=%C8%ED%F4%EE%F0%EC%E0%F6%E8%EE%ED%ED%FB%E9+%E1%FE%EB%EB%E5%F2%E5%ED%FC+%EE+%F1%E8%F2%F3%E0%F6%E8%E8+%E8+%EF%F0%E8%ED%E8%EC%E0%E5%EC%FB%F5+%EC%E5%F0%E0%F5+%EF%EE+%ED%E5%E4%EE%EF%F3%F9%E5%ED%E8%FE+%F0%E0%F1%EF%F0%EE%F1%F2%F0%E0%ED%E5%ED%E8%FF+%E7%E0%E1%EE%EB%E5%E2%E0%ED%E8%E9%2C+%E2%FB%E7%E2%E0%ED%ED%FB%F5+%ED%EE%E2%FB%EC+%EA%EE%F0%EE%ED%E0%E2%E8%F0%F3%F1%EE%EC&amp;where=&amp;how=d&amp;from=&amp;to="/>
+    <hyperlink ref="C134" r:id="rId25"/>
+    <hyperlink ref="C159" r:id="rId26"/>
+    <hyperlink ref="F173" r:id="rId27" display="https://www.gub.uy/sistema-nacional-emergencias/comunicacion/comunicados/informe-situacion-sobre-coronavirus-covid-19-uruguay-DATE"/>
+    <hyperlink ref="C7:K7" r:id="rId28" display="https://www.argentina.gob.ar/coronavirus/informes-diarios/reportes/diciembre2020"/>
+    <hyperlink ref="C2" r:id="rId29" location="/" display="http://covid.moph-dw.org/ - /"/>
+    <hyperlink ref="C107" r:id="rId30"/>
+    <hyperlink ref="C124" r:id="rId31"/>
+    <hyperlink ref="C126" r:id="rId32"/>
+    <hyperlink ref="C138" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>

</xml_diff>